<commit_message>
update test for regulus
</commit_message>
<xml_diff>
--- a/regulus/test/fuction_test.xlsx
+++ b/regulus/test/fuction_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>テスト項目</t>
     <rPh sb="3" eb="5">
@@ -44,53 +44,31 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>Query</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Body</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Path</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>1.0.0</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Webページにアクセス</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Path</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Query</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Body</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Path</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1.0.0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>currencies_usd: [&lt;USDJPYの通貨情報&gt;]
-currencies_eur: [&lt;EURJPYの通貨情報&gt;]
-currencies_gbp: [&lt;GBPJPYの通貨情報&gt;]</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -105,11 +83,50 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Function</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Webページにアクセス</t>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;div id="tweet"&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;div id="article"&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.1.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rates: [&lt;USDJPYの通貨情報&gt;]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rates: [&lt;USDJPYの通貨情報&gt;]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テスト対象</t>
+    <rPh sb="3" eb="5">
+      <t>タイショウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -117,10 +134,70 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>Controller</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Controller</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Controller</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>View</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>1.1.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>View</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>View</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Method</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RatesController#show</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RatesController#update</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TweetsController#show</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TweetsController#update</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ArticlesController#show</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ArticlesController#update</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RatesController#show</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TweetsController#show</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>-</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -129,110 +206,19 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>View</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;div id="currency"&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;div id="tweet"&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;div id="article"&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/tweet</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/article</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: ok</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/rate</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/rate</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/tweet</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/article</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>1.0.0</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;div id="currency"&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>View</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Webページにアクセス</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>1.1.0</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>1.1.0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>通貨情報取得</t>
-    <rPh sb="0" eb="4">
-      <t>ツウカジョウホウ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>シュトク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ツイート取得</t>
-    <rPh sb="4" eb="6">
-      <t>シュトク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>日経記事取得</t>
-    <rPh sb="0" eb="4">
-      <t>ニッケイキジ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>シュトク</t>
-    </rPh>
+    <t>tweets: [&lt;ツイート&gt;]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;div id="rate"&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1046,24 +1032,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I10"/>
+  <dimension ref="B1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.1640625" customWidth="1"/>
-    <col min="4" max="4" width="37.83203125" customWidth="1"/>
-    <col min="5" max="5" width="9.5" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" customWidth="1"/>
-    <col min="7" max="8" width="40.1640625" customWidth="1"/>
-    <col min="9" max="9" width="47.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
+    <col min="6" max="7" width="40.1640625" customWidth="1"/>
+    <col min="8" max="8" width="47.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="19" thickBot="1"/>
-    <row r="2" spans="2:9" ht="19" thickBot="1">
+    <row r="1" spans="2:8" ht="19" thickBot="1"/>
+    <row r="2" spans="2:8" ht="19" thickBot="1">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1071,230 +1056,226 @@
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:8">
       <c r="B3" s="16">
         <v>1</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>30</v>
+        <v>7</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="44">
+    <row r="4" spans="2:8">
       <c r="B4" s="24">
         <v>2</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="28" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:8">
       <c r="B5" s="29">
         <v>3</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="33" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:8">
       <c r="B6" s="24">
         <v>4</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="28" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:8">
       <c r="B7" s="29">
         <v>5</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="33" t="s">
-        <v>38</v>
+        <v>19</v>
+      </c>
+      <c r="H7" s="33" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:8">
       <c r="B8" s="29">
         <v>6</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="33" t="s">
-        <v>25</v>
+        <v>7</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:8">
       <c r="B9" s="29">
         <v>7</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="33" t="s">
-        <v>26</v>
+        <v>42</v>
+      </c>
+      <c r="H9" s="33" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="19" thickBot="1">
-      <c r="B10" s="20">
+    <row r="10" spans="2:8">
+      <c r="B10" s="29">
         <v>8</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="23" t="s">
-        <v>27</v>
+      <c r="C10" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="19" thickBot="1">
+      <c r="B11" s="20">
+        <v>9</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1340,13 +1321,13 @@
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>1</v>

</xml_diff>